<commit_message>
fix import charge + partner catalogue
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/CatalogueManagement/eFMS.API.Catalogue/Resources/Files/PartnerImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/CatalogueManagement/eFMS.API.Catalogue/Resources/Files/PartnerImportTemplate.xlsx
@@ -60,48 +60,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
-    <t>Taxcode</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Name Abr</t>
-  </si>
-  <si>
-    <t>Name EN</t>
-  </si>
-  <si>
-    <t>Name Local</t>
-  </si>
-  <si>
     <t>Contact Person</t>
   </si>
   <si>
     <t>Phone</t>
   </si>
   <si>
-    <t xml:space="preserve"> City </t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>Zipcode</t>
   </si>
   <si>
-    <t>Billing Address Local</t>
-  </si>
-  <si>
-    <t>Billing  Address EN</t>
-  </si>
-  <si>
-    <t>Shipping  Address EN</t>
-  </si>
-  <si>
-    <t>Shipping Address Local</t>
-  </si>
-  <si>
     <t xml:space="preserve">Email </t>
   </si>
   <si>
@@ -127,6 +94,39 @@
   </si>
   <si>
     <t>ABC</t>
+  </si>
+  <si>
+    <t>Name Abr(*)</t>
+  </si>
+  <si>
+    <t>Name EN(*)</t>
+  </si>
+  <si>
+    <t>Name Local(*)</t>
+  </si>
+  <si>
+    <t>Taxcode(*)</t>
+  </si>
+  <si>
+    <t>Category(*)</t>
+  </si>
+  <si>
+    <t>Billing  Address EN(*)</t>
+  </si>
+  <si>
+    <t>Billing Address Local(*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> City (*)</t>
+  </si>
+  <si>
+    <t>Country(*)</t>
+  </si>
+  <si>
+    <t>Shipping  Address EN(*)</t>
+  </si>
+  <si>
+    <t>Shipping Address Local(*)</t>
   </si>
 </sst>
 </file>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -525,79 +525,79 @@
   <sheetData>
     <row r="1" spans="1:25" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="M1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="S1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="U1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="V1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y1" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
@@ -611,7 +611,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>

</xml_diff>